<commit_message>
added feature for right nav
</commit_message>
<xml_diff>
--- a/src/test/resources/orProperties.xlsx
+++ b/src/test/resources/orProperties.xlsx
@@ -536,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D2" sqref="D2:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -547,10 +547,11 @@
     <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -561,7 +562,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -571,8 +572,12 @@
       <c r="C2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="str">
+        <f>CONCATENATE(A2,"=",B2,"~",C2)</f>
+        <v>txtUsername=id~LoginUserName</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -582,8 +587,12 @@
       <c r="C3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D20" si="0">CONCATENATE(A3,"=",B3,"~",C3)</f>
+        <v>txtPassword=id~LoginPassword</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -593,8 +602,12 @@
       <c r="C4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>btnLogin=xpath~//button[@type='submit']</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -604,8 +617,12 @@
       <c r="C5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>txtName=name~name</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -615,8 +632,12 @@
       <c r="C6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>btnSubmit=xpath~//button[contains(text(),'Submit')]</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -626,8 +647,12 @@
       <c r="C7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>txtEmail=name~email</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -637,8 +662,12 @@
       <c r="C8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>txtPhone=name~phone</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -648,8 +677,12 @@
       <c r="C9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>txtTollFreeNumber=name~tollFreeNumber</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -659,8 +692,12 @@
       <c r="C10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>txtDescription=name~description</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -670,8 +707,12 @@
       <c r="C11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>txtHours=name~hours</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -681,8 +722,12 @@
       <c r="C12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>txtWebsite=name~website</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -692,8 +737,12 @@
       <c r="C13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>txtGroupType=name~groupType</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -703,8 +752,12 @@
       <c r="C14" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>txtParentName=name~parentName</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -714,8 +767,12 @@
       <c r="C15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>txtCity=name~city</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -725,8 +782,12 @@
       <c r="C16" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>txtState=name~state</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -736,8 +797,12 @@
       <c r="C17" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>tblTable=xpath~.//*[@id='container']//tr</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -747,8 +812,12 @@
       <c r="C18" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>tblpagination=xpath~//*[@class='pagination ng-table-pagination pull-left']</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>43</v>
       </c>
@@ -758,8 +827,12 @@
       <c r="C19" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>btnRightNav=xpath~//a[@ng-click='toggleOffsidebarVisible()']</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -768,6 +841,10 @@
       </c>
       <c r="C20" t="s">
         <v>46</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>lstRightnavAcc=xpath~//*[@class='panel-body box-tree']//span</v>
       </c>
     </row>
   </sheetData>

</xml_diff>